<commit_message>
Modified the dates for expected start and finish date on the project proposal to calculate the current year and add 1 so that we don't have to update the script when the new year happens, it will always be current year + 1
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Redesigned the AI steps as sometimes the PPM application freezes the browser at the same time that the AI is trying to click
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Modified reporter event error text to be more accurate
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
pdated setting the Region value to be traditional OR, the validation process of PPM can cause the value not to be accepted by the UI when we do the AI type
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -520,15 +520,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Added another .sync statement
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Made the ClickLoop function, replaced duplicative code throughout with references to ClickLoop, made the proposal search as a function, so as to allow easy sharing with other scripts.
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Updated PPMProposalSearch function to look for the text Saved Searches to know Search click worked and commented .sync after that to prevent PPM from auto closing the menu popup
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Removed unused function Added function comments
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Found another example where the PPM application sometimes locks up, click statement with CLickLoop call
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Modified the ClickLoop retry counter to be 3 instead of 90
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Updated to handle 15.0.2 changes.  Script should still work on 15.0.1 as well.
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Updated to take advantage of additional capabilities in 15.0.2 around object recognition.  This will no longer properly run on 15.0.1.
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-business-case/Default.xlsx
+++ b/uft-one-ppm-build-business-case/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>